<commit_message>
Add late MBLD result for Yuichi Hamada
</commit_message>
<xml_diff>
--- a/data/2021-06-14/SCW Weekly Comp 2021-06-14 (Responses).xlsx
+++ b/data/2021-06-14/SCW Weekly Comp 2021-06-14 (Responses).xlsx
@@ -1,19 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\mike\projects\work\scw-comp\data\2021-06-14\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45AAC3AB-093B-40C6-A0F0-7B389A158430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Form Responses 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Form Responses 1'!$A$1:$DL$166</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Form Responses 1'!$A$1:$DL$166</definedName>
   </definedNames>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="257">
   <si>
     <t>Timestamp</t>
   </si>
@@ -772,75 +782,102 @@
   </si>
   <si>
     <t>1:33.47</t>
+  </si>
+  <si>
+    <t>Yuichi Hamada</t>
+  </si>
+  <si>
+    <t>2012HAMA02</t>
+  </si>
+  <si>
+    <t>https://m.facebook.com/events/1486483778369091?view=permalink&amp;id=1490555891295213</t>
+  </si>
+  <si>
+    <t>55:24</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf quotePrefix="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+  <cellXfs count="11">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1030,26 +1067,29 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:DF68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView tabSelected="1" topLeftCell="CU1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="CU68" sqref="A68:XFD68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="116" width="21.57"/>
+    <col min="1" max="116" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1381,9 +1421,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>44364.90381059027</v>
+        <v>44364.903810590273</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>19</v>
@@ -1422,9 +1462,9 @@
         <v>13.86</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
-        <v>44364.96005513889</v>
+        <v>44364.960055138887</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>24</v>
@@ -1442,24 +1482,24 @@
         <v>27</v>
       </c>
       <c r="CJ3" s="3">
-        <v>33.0</v>
+        <v>33</v>
       </c>
       <c r="CK3" s="3">
-        <v>33.0</v>
+        <v>33</v>
       </c>
       <c r="CL3" s="3">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="CM3" s="3">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="CN3" s="3">
-        <v>31.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>44365.88316453704</v>
+        <v>44365.883164537037</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>28</v>
@@ -1480,22 +1520,22 @@
         <v>32</v>
       </c>
       <c r="CJ4" s="3">
-        <v>29.0</v>
+        <v>29</v>
       </c>
       <c r="CK4" s="3">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="CL4" s="3" t="s">
         <v>33</v>
       </c>
       <c r="CM4" s="3">
-        <v>29.0</v>
+        <v>29</v>
       </c>
       <c r="CN4" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>44367.51496148148</v>
       </c>
@@ -1536,9 +1576,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>44367.51552111111</v>
+        <v>44367.515521111112</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>34</v>
@@ -1577,9 +1617,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
-        <v>44367.5163069213</v>
+        <v>44367.516306921301</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>34</v>
@@ -1606,21 +1646,21 @@
         <v>20.13</v>
       </c>
       <c r="R7" s="3">
-        <v>19.17</v>
+        <v>19.170000000000002</v>
       </c>
       <c r="S7" s="3">
-        <v>19.35</v>
+        <v>19.350000000000001</v>
       </c>
       <c r="T7" s="3">
-        <v>19.17</v>
+        <v>19.170000000000002</v>
       </c>
       <c r="U7" s="3">
         <v>19.73</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>44367.51712495371</v>
+        <v>44367.517124953709</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>34</v>
@@ -1659,7 +1699,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>44367.51791461806</v>
       </c>
@@ -1700,7 +1740,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>44368.089386527776</v>
       </c>
@@ -1726,18 +1766,18 @@
         <v>33</v>
       </c>
       <c r="CL10" s="3">
-        <v>42.0</v>
+        <v>42</v>
       </c>
       <c r="CM10" s="3">
-        <v>42.0</v>
+        <v>42</v>
       </c>
       <c r="CN10" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <v>44368.09284280092</v>
+        <v>44368.092842800921</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>65</v>
@@ -1755,16 +1795,16 @@
         <v>69</v>
       </c>
       <c r="DD11" s="3">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="DE11" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="DF11" s="5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>44368.441341990736</v>
       </c>
@@ -1805,7 +1845,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>44368.517416250004</v>
       </c>
@@ -1825,13 +1865,13 @@
         <v>83</v>
       </c>
       <c r="BV13" s="3">
-        <v>33.38</v>
+        <v>33.380000000000003</v>
       </c>
       <c r="BW13" s="3">
         <v>53.56</v>
       </c>
       <c r="BX13" s="3">
-        <v>40.77</v>
+        <v>40.770000000000003</v>
       </c>
       <c r="BY13" s="3">
         <v>37.74</v>
@@ -1840,15 +1880,15 @@
         <v>48.88</v>
       </c>
       <c r="CA13" s="3">
-        <v>33.38</v>
+        <v>33.380000000000003</v>
       </c>
       <c r="CB13" s="3">
         <v>42.46</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
-        <v>44368.51882134259</v>
+        <v>44368.518821342594</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>80</v>
@@ -1869,10 +1909,10 @@
         <v>41.99</v>
       </c>
       <c r="AU14" s="3">
-        <v>36.45</v>
+        <v>36.450000000000003</v>
       </c>
       <c r="AV14" s="3">
-        <v>39.8</v>
+        <v>39.799999999999997</v>
       </c>
       <c r="AW14" s="3">
         <v>29.99</v>
@@ -1887,7 +1927,7 @@
         <v>36.5</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>44368.519381122685</v>
       </c>
@@ -1925,12 +1965,12 @@
         <v>14.98</v>
       </c>
       <c r="U15" s="3">
-        <v>16.4</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>16.399999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
-        <v>44368.71525790509</v>
+        <v>44368.715257905089</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>87</v>
@@ -1948,10 +1988,10 @@
         <v>89</v>
       </c>
       <c r="O16" s="3">
-        <v>18.08</v>
+        <v>18.079999999999998</v>
       </c>
       <c r="P16" s="3">
-        <v>16.92</v>
+        <v>16.920000000000002</v>
       </c>
       <c r="Q16" s="3">
         <v>21.12</v>
@@ -1963,15 +2003,15 @@
         <v>21.17</v>
       </c>
       <c r="T16" s="3">
-        <v>16.92</v>
+        <v>16.920000000000002</v>
       </c>
       <c r="U16" s="3">
         <v>19.5</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
-        <v>44368.97700375</v>
+        <v>44368.977003749998</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>19</v>
@@ -1989,7 +2029,7 @@
         <v>90</v>
       </c>
       <c r="O17" s="3">
-        <v>32.91</v>
+        <v>32.909999999999997</v>
       </c>
       <c r="P17" s="3">
         <v>34.75</v>
@@ -2010,9 +2050,9 @@
         <v>29.58</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
-        <v>44368.99205563657</v>
+        <v>44368.992055636569</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>19</v>
@@ -2051,9 +2091,9 @@
         <v>21.55</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>44369.03776229167</v>
+        <v>44369.037762291671</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>19</v>
@@ -2071,10 +2111,10 @@
         <v>94</v>
       </c>
       <c r="H19" s="3">
-        <v>4.86</v>
+        <v>4.8600000000000003</v>
       </c>
       <c r="I19" s="3">
-        <v>9.21</v>
+        <v>9.2100000000000009</v>
       </c>
       <c r="J19" s="3">
         <v>7.21</v>
@@ -2086,13 +2126,13 @@
         <v>8.34</v>
       </c>
       <c r="M19" s="3">
-        <v>4.86</v>
+        <v>4.8600000000000003</v>
       </c>
       <c r="N19" s="3">
         <v>7.82</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>44369.449183460645</v>
       </c>
@@ -2127,9 +2167,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
-        <v>44369.76405629629</v>
+        <v>44369.764056296292</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>101</v>
@@ -2147,7 +2187,7 @@
         <v>103</v>
       </c>
       <c r="CJ21" s="3">
-        <v>54.0</v>
+        <v>54</v>
       </c>
       <c r="CK21" s="3" t="s">
         <v>41</v>
@@ -2156,15 +2196,15 @@
         <v>41</v>
       </c>
       <c r="CM21" s="3">
-        <v>54.0</v>
+        <v>54</v>
       </c>
       <c r="CN21" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <v>44369.89548236111</v>
+        <v>44369.895482361113</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>19</v>
@@ -2203,7 +2243,7 @@
         <v>11.84</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>44370.455495567134</v>
       </c>
@@ -2238,7 +2278,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>44370.529579988426</v>
       </c>
@@ -2273,7 +2313,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>44370.62483108796</v>
       </c>
@@ -2308,9 +2348,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
-        <v>44370.68493216435</v>
+        <v>44370.684932164353</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>87</v>
@@ -2343,9 +2383,9 @@
         <v>126</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
-        <v>44370.83529081018</v>
+        <v>44370.835290810181</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>127</v>
@@ -2363,24 +2403,24 @@
         <v>129</v>
       </c>
       <c r="CJ27" s="3">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="CK27" s="3">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="CL27" s="3">
-        <v>31.0</v>
+        <v>31</v>
       </c>
       <c r="CM27" s="3">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="CN27" s="3">
-        <v>29.0</v>
-      </c>
-    </row>
-    <row r="28">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
-        <v>44371.43802770833</v>
+        <v>44371.438027708333</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>71</v>
@@ -2419,9 +2459,9 @@
         <v>136</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
-        <v>44371.72624520834</v>
+        <v>44371.726245208338</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>87</v>
@@ -2460,9 +2500,9 @@
         <v>143</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
-        <v>44372.6491827662</v>
+        <v>44372.649182766203</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>144</v>
@@ -2483,24 +2523,24 @@
         <v>23.79</v>
       </c>
       <c r="BJ30" s="3">
-        <v>17.67</v>
+        <v>17.670000000000002</v>
       </c>
       <c r="BK30" s="3">
         <v>17.95</v>
       </c>
       <c r="BL30" s="3">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="BM30" s="3">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="BN30" s="3">
         <v>19.14</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
-        <v>44372.65019973379</v>
+        <v>44372.650199733791</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>144</v>
@@ -2527,18 +2567,18 @@
         <v>21.53</v>
       </c>
       <c r="BS31" s="3">
-        <v>32.2</v>
+        <v>32.200000000000003</v>
       </c>
       <c r="BT31" s="3">
         <v>15.25</v>
       </c>
       <c r="BU31" s="3">
-        <v>18.85</v>
-      </c>
-    </row>
-    <row r="32">
+        <v>18.850000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:97" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
-        <v>44372.65155958333</v>
+        <v>44372.651559583333</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>144</v>
@@ -2574,9 +2614,9 @@
         <v>151</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
-        <v>44372.65280813657</v>
+        <v>44372.652808136569</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>144</v>
@@ -2594,7 +2634,7 @@
         <v>25.79</v>
       </c>
       <c r="CD33" s="3">
-        <v>34.45</v>
+        <v>34.450000000000003</v>
       </c>
       <c r="CE33" s="3">
         <v>28.13</v>
@@ -2612,9 +2652,9 @@
         <v>26.22</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
-        <v>44372.65392972222</v>
+        <v>44372.653929722219</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>144</v>
@@ -2635,7 +2675,7 @@
         <v>8.15</v>
       </c>
       <c r="J34" s="3">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="K34" s="3">
         <v>7.72</v>
@@ -2647,12 +2687,12 @@
         <v>4.79</v>
       </c>
       <c r="N34" s="3">
-        <v>8.96</v>
-      </c>
-    </row>
-    <row r="35">
+        <v>8.9600000000000009</v>
+      </c>
+    </row>
+    <row r="35" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
-        <v>44372.65497469908</v>
+        <v>44372.654974699079</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>144</v>
@@ -2676,19 +2716,19 @@
         <v>18.59</v>
       </c>
       <c r="R35" s="3">
-        <v>17.9</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="S35" s="3">
-        <v>18.67</v>
+        <v>18.670000000000002</v>
       </c>
       <c r="T35" s="3">
-        <v>17.9</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="U35" s="3">
         <v>18.54</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>44372.655974884256</v>
       </c>
@@ -2726,9 +2766,9 @@
         <v>159</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
-        <v>44372.65730018519</v>
+        <v>44372.657300185187</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>144</v>
@@ -2764,9 +2804,9 @@
         <v>166</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
-        <v>44372.65840247685</v>
+        <v>44372.658402476853</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>144</v>
@@ -2802,7 +2842,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>44372.65936982639</v>
       </c>
@@ -2834,7 +2874,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>44373.08630299769</v>
       </c>
@@ -2857,7 +2897,7 @@
         <v>22.89</v>
       </c>
       <c r="P40" s="3">
-        <v>20.44</v>
+        <v>20.440000000000001</v>
       </c>
       <c r="Q40" s="3">
         <v>19.8</v>
@@ -2875,7 +2915,7 @@
         <v>20.09</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>44373.087062708335</v>
       </c>
@@ -2910,9 +2950,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
-        <v>44373.70569482639</v>
+        <v>44373.705694826393</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>181</v>
@@ -2930,16 +2970,16 @@
         <v>183</v>
       </c>
       <c r="DD42" s="3">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="DE42" s="3">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="DF42" s="5" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>44374.05993106481</v>
       </c>
@@ -2974,7 +3014,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>44374.310195162034</v>
       </c>
@@ -3012,9 +3052,9 @@
         <v>24.84</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
-        <v>44374.42603614583</v>
+        <v>44374.426036145829</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>34</v>
@@ -3032,24 +3072,24 @@
         <v>188</v>
       </c>
       <c r="CJ45" s="3">
-        <v>46.0</v>
+        <v>46</v>
       </c>
       <c r="CK45" s="3">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="CL45" s="3">
-        <v>34.0</v>
+        <v>34</v>
       </c>
       <c r="CM45" s="3">
-        <v>34.0</v>
+        <v>34</v>
       </c>
       <c r="CN45" s="3">
-        <v>40.0</v>
-      </c>
-    </row>
-    <row r="46">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="46" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
-        <v>44374.56307636574</v>
+        <v>44374.563076365739</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>87</v>
@@ -3088,9 +3128,9 @@
         <v>194</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
-        <v>44374.58815700232</v>
+        <v>44374.588157002319</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>195</v>
@@ -3129,9 +3169,9 @@
         <v>27.62</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
-        <v>44374.71570973379</v>
+        <v>44374.715709733791</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>80</v>
@@ -3167,9 +3207,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
-        <v>44374.73746049769</v>
+        <v>44374.737460497687</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>202</v>
@@ -3205,9 +3245,9 @@
         <v>11.22</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
-        <v>44374.73832888889</v>
+        <v>44374.738328888889</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>202</v>
@@ -3243,9 +3283,9 @@
         <v>41.25</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
-        <v>44374.83284157407</v>
+        <v>44374.832841574069</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>71</v>
@@ -3284,7 +3324,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>44374.848999803246</v>
       </c>
@@ -3316,18 +3356,18 @@
         <v>18.46</v>
       </c>
       <c r="S52" s="3">
-        <v>16.92</v>
+        <v>16.920000000000002</v>
       </c>
       <c r="T52" s="3">
         <v>14.61</v>
       </c>
       <c r="U52" s="3">
-        <v>16.44</v>
-      </c>
-    </row>
-    <row r="53">
+        <v>16.440000000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
-        <v>44374.86269045139</v>
+        <v>44374.862690451388</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>71</v>
@@ -3357,7 +3397,7 @@
         <v>213</v>
       </c>
       <c r="AX53" s="3">
-        <v>32.27</v>
+        <v>32.270000000000003</v>
       </c>
       <c r="AY53" s="3">
         <v>28.14</v>
@@ -3366,7 +3406,7 @@
         <v>31.08</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>44375.073382476854</v>
       </c>
@@ -3407,9 +3447,9 @@
         <v>24.69</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
-        <v>44375.07494702547</v>
+        <v>44375.074947025467</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>214</v>
@@ -3448,9 +3488,9 @@
         <v>11.95</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
-        <v>44375.07636908565</v>
+        <v>44375.076369085647</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>214</v>
@@ -3489,7 +3529,7 @@
         <v>9.09</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>44375.078245902776</v>
       </c>
@@ -3530,7 +3570,7 @@
         <v>25.9</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>44375.080093819444</v>
       </c>
@@ -3571,9 +3611,9 @@
         <v>224</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
-        <v>44375.16240332176</v>
+        <v>44375.162403321759</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>225</v>
@@ -3600,7 +3640,7 @@
         <v>13.96</v>
       </c>
       <c r="BK59" s="3">
-        <v>8.8</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="BL59" s="3">
         <v>7.8</v>
@@ -3612,9 +3652,9 @@
         <v>8.34</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
-        <v>44375.16330100695</v>
+        <v>44375.163301006949</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>225</v>
@@ -3641,7 +3681,7 @@
         <v>15.12</v>
       </c>
       <c r="R60" s="3">
-        <v>16.24</v>
+        <v>16.239999999999998</v>
       </c>
       <c r="S60" s="3">
         <v>13.57</v>
@@ -3653,9 +3693,9 @@
         <v>14.18</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
-        <v>44375.16425778935</v>
+        <v>44375.164257789351</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>225</v>
@@ -3679,7 +3719,7 @@
         <v>4.97</v>
       </c>
       <c r="J61" s="3">
-        <v>4.61</v>
+        <v>4.6100000000000003</v>
       </c>
       <c r="K61" s="3">
         <v>5.19</v>
@@ -3694,7 +3734,7 @@
         <v>4.92</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>44375.16573630787</v>
       </c>
@@ -3735,7 +3775,7 @@
         <v>58.05</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>44375.1665315625</v>
       </c>
@@ -3776,9 +3816,9 @@
         <v>239</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
-        <v>44375.20294280093</v>
+        <v>44375.202942800926</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>225</v>
@@ -3811,9 +3851,9 @@
         <v>244</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
-        <v>44375.20396596065</v>
+        <v>44375.203965960653</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>225</v>
@@ -3843,7 +3883,7 @@
         <v>12.78</v>
       </c>
       <c r="CG65" s="3">
-        <v>17.85</v>
+        <v>17.850000000000001</v>
       </c>
       <c r="CH65" s="3">
         <v>12.06</v>
@@ -3852,9 +3892,9 @@
         <v>12.84</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:110" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
-        <v>44375.21646130787</v>
+        <v>44375.216461307871</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>225</v>
@@ -3893,75 +3933,106 @@
         <v>252</v>
       </c>
     </row>
+    <row r="67" spans="1:110" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A67" s="6">
+        <v>44375.680598935185</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F67" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="DD67" s="1">
+        <v>11</v>
+      </c>
+      <c r="DE67" s="1">
+        <v>10</v>
+      </c>
+      <c r="DF67" s="9" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="68" spans="1:110" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <autoFilter ref="$A$1:$DL$166"/>
+  <autoFilter ref="A1:DL166" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="F2"/>
-    <hyperlink r:id="rId2" ref="F3"/>
-    <hyperlink r:id="rId3" ref="F4"/>
-    <hyperlink r:id="rId4" ref="F5"/>
-    <hyperlink r:id="rId5" ref="F6"/>
-    <hyperlink r:id="rId6" ref="F7"/>
-    <hyperlink r:id="rId7" ref="F8"/>
-    <hyperlink r:id="rId8" ref="F9"/>
-    <hyperlink r:id="rId9" ref="F10"/>
-    <hyperlink r:id="rId10" ref="F11"/>
-    <hyperlink r:id="rId11" ref="F12"/>
-    <hyperlink r:id="rId12" ref="F13"/>
-    <hyperlink r:id="rId13" ref="F14"/>
-    <hyperlink r:id="rId14" ref="F15"/>
-    <hyperlink r:id="rId15" ref="F16"/>
-    <hyperlink r:id="rId16" ref="F17"/>
-    <hyperlink r:id="rId17" ref="F18"/>
-    <hyperlink r:id="rId18" ref="F19"/>
-    <hyperlink r:id="rId19" ref="F20"/>
-    <hyperlink r:id="rId20" ref="F21"/>
-    <hyperlink r:id="rId21" ref="F22"/>
-    <hyperlink r:id="rId22" ref="F23"/>
-    <hyperlink r:id="rId23" ref="F24"/>
-    <hyperlink r:id="rId24" ref="F25"/>
-    <hyperlink r:id="rId25" ref="F26"/>
-    <hyperlink r:id="rId26" ref="F27"/>
-    <hyperlink r:id="rId27" ref="F28"/>
-    <hyperlink r:id="rId28" ref="F29"/>
-    <hyperlink r:id="rId29" ref="F30"/>
-    <hyperlink r:id="rId30" ref="F31"/>
-    <hyperlink r:id="rId31" ref="F32"/>
-    <hyperlink r:id="rId32" ref="F33"/>
-    <hyperlink r:id="rId33" ref="F34"/>
-    <hyperlink r:id="rId34" ref="F35"/>
-    <hyperlink r:id="rId35" ref="F36"/>
-    <hyperlink r:id="rId36" ref="F37"/>
-    <hyperlink r:id="rId37" ref="F38"/>
-    <hyperlink r:id="rId38" ref="F39"/>
-    <hyperlink r:id="rId39" ref="F40"/>
-    <hyperlink r:id="rId40" ref="F41"/>
-    <hyperlink r:id="rId41" ref="F42"/>
-    <hyperlink r:id="rId42" ref="F43"/>
-    <hyperlink r:id="rId43" ref="F44"/>
-    <hyperlink r:id="rId44" ref="F45"/>
-    <hyperlink r:id="rId45" ref="F46"/>
-    <hyperlink r:id="rId46" ref="F47"/>
-    <hyperlink r:id="rId47" ref="F48"/>
-    <hyperlink r:id="rId48" ref="F49"/>
-    <hyperlink r:id="rId49" ref="F50"/>
-    <hyperlink r:id="rId50" ref="F51"/>
-    <hyperlink r:id="rId51" ref="F52"/>
-    <hyperlink r:id="rId52" ref="F53"/>
-    <hyperlink r:id="rId53" ref="F54"/>
-    <hyperlink r:id="rId54" ref="F55"/>
-    <hyperlink r:id="rId55" ref="F56"/>
-    <hyperlink r:id="rId56" ref="F57"/>
-    <hyperlink r:id="rId57" ref="F58"/>
-    <hyperlink r:id="rId58" ref="F59"/>
-    <hyperlink r:id="rId59" ref="F60"/>
-    <hyperlink r:id="rId60" ref="F61"/>
-    <hyperlink r:id="rId61" ref="F62"/>
-    <hyperlink r:id="rId62" ref="F63"/>
-    <hyperlink r:id="rId63" ref="F64"/>
-    <hyperlink r:id="rId64" ref="F65"/>
-    <hyperlink r:id="rId65" ref="F66"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="F7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="F8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="F9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="F10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="F11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="F12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="F13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="F14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="F15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="F16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="F17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="F18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="F19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="F20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="F21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="F22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="F23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="F24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="F25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="F26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="F27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="F28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="F29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="F30" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="F31" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="F32" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="F33" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="F34" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="F35" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="F36" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="F37" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="F38" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="F39" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="F40" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="F41" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="F42" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="F43" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="F44" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="F45" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="F46" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="F47" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="F48" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="F49" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="F50" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="F51" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="F52" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="F53" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="F54" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="F55" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="F56" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="F57" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="F58" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="F59" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="F60" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="F61" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="F62" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="F63" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="F64" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="F65" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="F66" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="F67" r:id="rId66" xr:uid="{0675CAAC-00F2-49BE-A082-44152B4334B4}"/>
   </hyperlinks>
-  <drawing r:id="rId66"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>